<commit_message>
Remove last empty character.
</commit_message>
<xml_diff>
--- a/Testing_Case_Calculation/src/D-Link-Wi-Fi-config_time_for_tool.xlsx
+++ b/Testing_Case_Calculation/src/D-Link-Wi-Fi-config_time_for_tool.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryantliu/KobeDevNodeProject/Leslie_Wish_Tool/Testing_Case_Calculation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryantliu/KobeDevNodeProject/Leslie_Wish_Tool/Testing_Case_Calculation/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="1780" windowWidth="30120" windowHeight="17260" tabRatio="828" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200" tabRatio="828" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Record" sheetId="4" state="hidden" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="315">
   <si>
     <t xml:space="preserve">1. Input D-Link WiFi APP Ver. :                                          </t>
   </si>
@@ -1137,9 +1137,6 @@
     <t>D-Link DeFend regression function</t>
   </si>
   <si>
-    <t xml:space="preserve">Easy </t>
-  </si>
-  <si>
     <t>Full Total</t>
   </si>
   <si>
@@ -1150,6 +1147,30 @@
   </si>
   <si>
     <t>FOTA In Wizard</t>
+  </si>
+  <si>
+    <t>wizard</t>
+  </si>
+  <si>
+    <t>mesh compatibility</t>
+  </si>
+  <si>
+    <t>Advance parental control</t>
+  </si>
+  <si>
+    <t>Parental control</t>
+  </si>
+  <si>
+    <t>Remote management</t>
+  </si>
+  <si>
+    <t>D-Link DeFend full function</t>
+  </si>
+  <si>
+    <t>FOTA in wizard</t>
+  </si>
+  <si>
+    <t>Easy</t>
   </si>
 </sst>
 </file>
@@ -1796,7 +1817,7 @@
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1971,6 +1992,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2082,6 +2106,7 @@
     <xf numFmtId="0" fontId="10" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2441,7 +2466,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="93" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2449,19 +2474,19 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="93"/>
+      <c r="A3" s="94"/>
       <c r="B3" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="93"/>
+      <c r="A4" s="94"/>
       <c r="B4" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="94" t="s">
+      <c r="A5" s="95" t="s">
         <v>45</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -2469,13 +2494,13 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="95"/>
+      <c r="A6" s="96"/>
       <c r="B6" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="96" t="s">
+      <c r="A7" s="97" t="s">
         <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2483,19 +2508,19 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="97"/>
+      <c r="A8" s="98"/>
       <c r="B8" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="97"/>
+      <c r="A9" s="98"/>
       <c r="B9" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="98" t="s">
+      <c r="A10" s="99" t="s">
         <v>55</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -2503,13 +2528,13 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="99"/>
+      <c r="A11" s="100"/>
       <c r="B11" s="8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="89" t="s">
         <v>58</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -2517,19 +2542,19 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="89"/>
+      <c r="A13" s="90"/>
       <c r="B13" s="9" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="89"/>
+      <c r="A14" s="90"/>
       <c r="B14" s="9" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="88" t="s">
+      <c r="A15" s="89" t="s">
         <v>78</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -2537,37 +2562,37 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="89"/>
+      <c r="A16" s="90"/>
       <c r="B16" s="9" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="89"/>
+      <c r="A17" s="90"/>
       <c r="B17" s="9" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="89"/>
+      <c r="A18" s="90"/>
       <c r="B18" s="9" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="89"/>
+      <c r="A19" s="90"/>
       <c r="B19" s="9" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="89"/>
+      <c r="A20" s="90"/>
       <c r="B20" s="11" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="90" t="s">
+      <c r="A21" s="91" t="s">
         <v>86</v>
       </c>
       <c r="B21" s="12" t="s">
@@ -2575,7 +2600,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="91"/>
+      <c r="A22" s="92"/>
       <c r="B22" s="13" t="s">
         <v>85</v>
       </c>
@@ -2608,12 +2633,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P918"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:XFD1048576"/>
       <selection pane="topRight" sqref="A1:XFD1048576"/>
       <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="O3" sqref="O3:O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -2631,81 +2656,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.3">
-      <c r="A1" s="114" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="107" t="s">
+      <c r="A1" s="115" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="116"/>
+      <c r="K1" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="108"/>
-      <c r="M1" s="108"/>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
+      <c r="N1" s="109"/>
+      <c r="O1" s="109"/>
+      <c r="P1" s="110"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.3">
-      <c r="A2" s="111" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="110"/>
-      <c r="L2" s="110"/>
-      <c r="M2" s="110"/>
-      <c r="N2" s="110"/>
-      <c r="O2" s="110"/>
-      <c r="P2" s="110"/>
+      <c r="A2" s="112" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="111"/>
+      <c r="O2" s="111"/>
+      <c r="P2" s="111"/>
     </row>
     <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="116" t="s">
+      <c r="A3" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="116"/>
-      <c r="C3" s="116" t="s">
+      <c r="B3" s="117"/>
+      <c r="C3" s="117" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="102" t="s">
+      <c r="D3" s="103" t="s">
         <v>119</v>
       </c>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="102"/>
-      <c r="K3" s="103" t="s">
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="103"/>
+      <c r="K3" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="103"/>
-      <c r="M3" s="103"/>
-      <c r="N3" s="103"/>
-      <c r="O3" s="106" t="s">
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="116" t="s">
+      <c r="P3" s="117" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:16" s="29" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="116"/>
-      <c r="B4" s="116"/>
-      <c r="C4" s="116"/>
+      <c r="A4" s="117"/>
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
       <c r="D4" s="27" t="s">
         <v>253</v>
       </c>
@@ -2739,14 +2764,14 @@
       <c r="N4" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="O4" s="106"/>
-      <c r="P4" s="116"/>
+      <c r="O4" s="107"/>
+      <c r="P4" s="117"/>
     </row>
     <row r="5" spans="1:16" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="30">
         <v>1</v>
       </c>
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="101" t="s">
         <v>180</v>
       </c>
       <c r="C5" s="31" t="s">
@@ -2804,12 +2829,12 @@
       <c r="A6" s="38">
         <v>2</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="39" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="40">
-        <f t="shared" ref="D5:D36" si="9">(INDEX(times1,MATCH(CONCATENATE($C6,"_Full"),model1,0),MATCH($D$4,plan1,0)))-SUM($E6:$I6)</f>
+        <f t="shared" ref="D6:D36" si="9">(INDEX(times1,MATCH(CONCATENATE($C6,"_Full"),model1,0),MATCH($D$4,plan1,0)))-SUM($E6:$I6)</f>
         <v>12.899999999999999</v>
       </c>
       <c r="E6" s="40">
@@ -2860,7 +2885,7 @@
       <c r="A7" s="38">
         <v>3</v>
       </c>
-      <c r="B7" s="100"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="44" t="s">
         <v>10</v>
       </c>
@@ -2916,7 +2941,7 @@
       <c r="A8" s="38">
         <v>4</v>
       </c>
-      <c r="B8" s="100"/>
+      <c r="B8" s="101"/>
       <c r="C8" s="44" t="s">
         <v>11</v>
       </c>
@@ -2972,7 +2997,7 @@
       <c r="A9" s="38">
         <v>5</v>
       </c>
-      <c r="B9" s="100"/>
+      <c r="B9" s="101"/>
       <c r="C9" s="44" t="s">
         <v>12</v>
       </c>
@@ -3028,7 +3053,7 @@
       <c r="A10" s="38">
         <v>6</v>
       </c>
-      <c r="B10" s="100"/>
+      <c r="B10" s="101"/>
       <c r="C10" s="44" t="s">
         <v>13</v>
       </c>
@@ -3084,7 +3109,7 @@
       <c r="A11" s="38">
         <v>7</v>
       </c>
-      <c r="B11" s="100"/>
+      <c r="B11" s="101"/>
       <c r="C11" s="44" t="s">
         <v>221</v>
       </c>
@@ -3140,7 +3165,7 @@
       <c r="A12" s="38">
         <v>8</v>
       </c>
-      <c r="B12" s="100"/>
+      <c r="B12" s="101"/>
       <c r="C12" s="44" t="s">
         <v>223</v>
       </c>
@@ -3196,7 +3221,7 @@
       <c r="A13" s="38">
         <v>9</v>
       </c>
-      <c r="B13" s="100"/>
+      <c r="B13" s="101"/>
       <c r="C13" s="39" t="s">
         <v>224</v>
       </c>
@@ -3212,8 +3237,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G13" s="40">
-        <f t="shared" si="2"/>
+      <c r="G13" s="88">
+        <f>INDEX(times1,MATCH(CONCATENATE($C13,"_Full"),model1,0),MATCH($G$4,plan1,0))</f>
         <v>0</v>
       </c>
       <c r="H13" s="40">
@@ -3252,7 +3277,7 @@
       <c r="A14" s="38">
         <v>10</v>
       </c>
-      <c r="B14" s="100"/>
+      <c r="B14" s="101"/>
       <c r="C14" s="46" t="s">
         <v>225</v>
       </c>
@@ -3308,7 +3333,7 @@
       <c r="A15" s="38">
         <v>11</v>
       </c>
-      <c r="B15" s="100"/>
+      <c r="B15" s="101"/>
       <c r="C15" s="46" t="s">
         <v>226</v>
       </c>
@@ -3364,7 +3389,7 @@
       <c r="A16" s="38">
         <v>12</v>
       </c>
-      <c r="B16" s="100"/>
+      <c r="B16" s="101"/>
       <c r="C16" s="47" t="s">
         <v>14</v>
       </c>
@@ -3385,7 +3410,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="40">
-        <f t="shared" si="3"/>
+        <f>INDEX(times1,MATCH(CONCATENATE($C16,"_Full"),model1,0),MATCH($H$4,plan1,0))</f>
         <v>0</v>
       </c>
       <c r="I16" s="40">
@@ -3420,7 +3445,7 @@
       <c r="A17" s="38">
         <v>13</v>
       </c>
-      <c r="B17" s="100"/>
+      <c r="B17" s="101"/>
       <c r="C17" s="47" t="s">
         <v>15</v>
       </c>
@@ -3476,7 +3501,7 @@
       <c r="A18" s="38">
         <v>14</v>
       </c>
-      <c r="B18" s="100"/>
+      <c r="B18" s="101"/>
       <c r="C18" s="44" t="s">
         <v>16</v>
       </c>
@@ -3532,7 +3557,7 @@
       <c r="A19" s="38">
         <v>15</v>
       </c>
-      <c r="B19" s="100"/>
+      <c r="B19" s="101"/>
       <c r="C19" s="49" t="s">
         <v>82</v>
       </c>
@@ -3588,7 +3613,7 @@
       <c r="A20" s="38">
         <v>16</v>
       </c>
-      <c r="B20" s="101"/>
+      <c r="B20" s="102"/>
       <c r="C20" s="49" t="s">
         <v>83</v>
       </c>
@@ -3644,7 +3669,7 @@
       <c r="A21" s="38">
         <v>17</v>
       </c>
-      <c r="B21" s="104" t="s">
+      <c r="B21" s="105" t="s">
         <v>227</v>
       </c>
       <c r="C21" s="50" t="s">
@@ -3702,7 +3727,7 @@
       <c r="A22" s="38">
         <v>18</v>
       </c>
-      <c r="B22" s="105"/>
+      <c r="B22" s="106"/>
       <c r="C22" s="51" t="s">
         <v>18</v>
       </c>
@@ -3758,7 +3783,7 @@
       <c r="A23" s="38">
         <v>19</v>
       </c>
-      <c r="B23" s="105"/>
+      <c r="B23" s="106"/>
       <c r="C23" s="51" t="s">
         <v>19</v>
       </c>
@@ -3814,7 +3839,7 @@
       <c r="A24" s="38">
         <v>20</v>
       </c>
-      <c r="B24" s="105"/>
+      <c r="B24" s="106"/>
       <c r="C24" s="51" t="s">
         <v>20</v>
       </c>
@@ -3870,7 +3895,7 @@
       <c r="A25" s="38">
         <v>21</v>
       </c>
-      <c r="B25" s="105"/>
+      <c r="B25" s="106"/>
       <c r="C25" s="53" t="s">
         <v>21</v>
       </c>
@@ -3926,7 +3951,7 @@
       <c r="A26" s="38">
         <v>22</v>
       </c>
-      <c r="B26" s="105"/>
+      <c r="B26" s="106"/>
       <c r="C26" s="51" t="s">
         <v>22</v>
       </c>
@@ -3982,7 +4007,7 @@
       <c r="A27" s="38">
         <v>23</v>
       </c>
-      <c r="B27" s="105"/>
+      <c r="B27" s="106"/>
       <c r="C27" s="53" t="s">
         <v>23</v>
       </c>
@@ -4038,7 +4063,7 @@
       <c r="A28" s="38">
         <v>24</v>
       </c>
-      <c r="B28" s="105"/>
+      <c r="B28" s="106"/>
       <c r="C28" s="51" t="s">
         <v>24</v>
       </c>
@@ -4094,7 +4119,7 @@
       <c r="A29" s="38">
         <v>25</v>
       </c>
-      <c r="B29" s="119" t="s">
+      <c r="B29" s="120" t="s">
         <v>88</v>
       </c>
       <c r="C29" s="54" t="s">
@@ -4152,7 +4177,7 @@
       <c r="A30" s="38">
         <v>26</v>
       </c>
-      <c r="B30" s="119"/>
+      <c r="B30" s="120"/>
       <c r="C30" s="54" t="s">
         <v>182</v>
       </c>
@@ -4208,7 +4233,7 @@
       <c r="A31" s="38">
         <v>27</v>
       </c>
-      <c r="B31" s="119"/>
+      <c r="B31" s="120"/>
       <c r="C31" s="55" t="s">
         <v>228</v>
       </c>
@@ -4264,7 +4289,7 @@
       <c r="A32" s="38">
         <v>28</v>
       </c>
-      <c r="B32" s="119"/>
+      <c r="B32" s="120"/>
       <c r="C32" s="55" t="s">
         <v>229</v>
       </c>
@@ -4320,7 +4345,7 @@
       <c r="A33" s="38">
         <v>29</v>
       </c>
-      <c r="B33" s="119"/>
+      <c r="B33" s="120"/>
       <c r="C33" s="55" t="s">
         <v>230</v>
       </c>
@@ -4376,7 +4401,7 @@
       <c r="A34" s="38">
         <v>30</v>
       </c>
-      <c r="B34" s="119"/>
+      <c r="B34" s="120"/>
       <c r="C34" s="55" t="s">
         <v>231</v>
       </c>
@@ -4432,7 +4457,7 @@
       <c r="A35" s="38">
         <v>31</v>
       </c>
-      <c r="B35" s="119"/>
+      <c r="B35" s="120"/>
       <c r="C35" s="56" t="s">
         <v>89</v>
       </c>
@@ -4488,7 +4513,7 @@
       <c r="A36" s="38">
         <v>32</v>
       </c>
-      <c r="B36" s="119"/>
+      <c r="B36" s="120"/>
       <c r="C36" s="58" t="s">
         <v>90</v>
       </c>
@@ -4544,7 +4569,7 @@
       <c r="A37" s="38">
         <v>33</v>
       </c>
-      <c r="B37" s="119"/>
+      <c r="B37" s="120"/>
       <c r="C37" s="58" t="s">
         <v>232</v>
       </c>
@@ -4600,7 +4625,7 @@
       <c r="A38" s="38">
         <v>34</v>
       </c>
-      <c r="B38" s="119"/>
+      <c r="B38" s="120"/>
       <c r="C38" s="58" t="s">
         <v>233</v>
       </c>
@@ -4656,7 +4681,7 @@
       <c r="A39" s="38">
         <v>35</v>
       </c>
-      <c r="B39" s="119"/>
+      <c r="B39" s="120"/>
       <c r="C39" s="58" t="s">
         <v>183</v>
       </c>
@@ -4712,7 +4737,7 @@
       <c r="A40" s="38">
         <v>36</v>
       </c>
-      <c r="B40" s="119"/>
+      <c r="B40" s="120"/>
       <c r="C40" s="58" t="s">
         <v>184</v>
       </c>
@@ -4768,7 +4793,7 @@
       <c r="A41" s="38">
         <v>37</v>
       </c>
-      <c r="B41" s="119"/>
+      <c r="B41" s="120"/>
       <c r="C41" s="58" t="s">
         <v>185</v>
       </c>
@@ -4824,7 +4849,7 @@
       <c r="A42" s="38">
         <v>38</v>
       </c>
-      <c r="B42" s="119"/>
+      <c r="B42" s="120"/>
       <c r="C42" s="58" t="s">
         <v>234</v>
       </c>
@@ -4880,7 +4905,7 @@
       <c r="A43" s="38">
         <v>39</v>
       </c>
-      <c r="B43" s="120" t="s">
+      <c r="B43" s="121" t="s">
         <v>25</v>
       </c>
       <c r="C43" s="59" t="s">
@@ -4938,7 +4963,7 @@
       <c r="A44" s="38">
         <v>40</v>
       </c>
-      <c r="B44" s="120"/>
+      <c r="B44" s="121"/>
       <c r="C44" s="59" t="s">
         <v>187</v>
       </c>
@@ -4994,7 +5019,7 @@
       <c r="A45" s="38">
         <v>41</v>
       </c>
-      <c r="B45" s="120"/>
+      <c r="B45" s="121"/>
       <c r="C45" s="60" t="s">
         <v>91</v>
       </c>
@@ -5050,7 +5075,7 @@
       <c r="A46" s="38">
         <v>42</v>
       </c>
-      <c r="B46" s="120"/>
+      <c r="B46" s="121"/>
       <c r="C46" s="39" t="s">
         <v>26</v>
       </c>
@@ -5104,7 +5129,7 @@
       <c r="A47" s="38">
         <v>43</v>
       </c>
-      <c r="B47" s="120"/>
+      <c r="B47" s="121"/>
       <c r="C47" s="39" t="s">
         <v>27</v>
       </c>
@@ -5158,7 +5183,7 @@
       <c r="A48" s="38">
         <v>44</v>
       </c>
-      <c r="B48" s="120"/>
+      <c r="B48" s="121"/>
       <c r="C48" s="39" t="s">
         <v>28</v>
       </c>
@@ -5214,7 +5239,7 @@
       <c r="A49" s="38">
         <v>45</v>
       </c>
-      <c r="B49" s="120"/>
+      <c r="B49" s="121"/>
       <c r="C49" s="39" t="s">
         <v>29</v>
       </c>
@@ -5268,7 +5293,7 @@
       <c r="A50" s="38">
         <v>46</v>
       </c>
-      <c r="B50" s="121"/>
+      <c r="B50" s="122"/>
       <c r="C50" s="60" t="s">
         <v>30</v>
       </c>
@@ -5324,7 +5349,7 @@
       <c r="A51" s="38">
         <v>47</v>
       </c>
-      <c r="B51" s="117" t="s">
+      <c r="B51" s="118" t="s">
         <v>31</v>
       </c>
       <c r="C51" s="61" t="s">
@@ -5380,7 +5405,7 @@
       <c r="A52" s="38">
         <v>48</v>
       </c>
-      <c r="B52" s="117"/>
+      <c r="B52" s="118"/>
       <c r="C52" s="61" t="s">
         <v>33</v>
       </c>
@@ -5434,7 +5459,7 @@
       <c r="A53" s="38">
         <v>49</v>
       </c>
-      <c r="B53" s="117"/>
+      <c r="B53" s="118"/>
       <c r="C53" s="61" t="s">
         <v>34</v>
       </c>
@@ -5488,7 +5513,7 @@
       <c r="A54" s="38">
         <v>50</v>
       </c>
-      <c r="B54" s="117"/>
+      <c r="B54" s="118"/>
       <c r="C54" s="62" t="s">
         <v>35</v>
       </c>
@@ -5542,7 +5567,7 @@
       <c r="A55" s="38">
         <v>51</v>
       </c>
-      <c r="B55" s="117"/>
+      <c r="B55" s="118"/>
       <c r="C55" s="63" t="s">
         <v>36</v>
       </c>
@@ -5596,7 +5621,7 @@
       <c r="A56" s="38">
         <v>52</v>
       </c>
-      <c r="B56" s="117"/>
+      <c r="B56" s="118"/>
       <c r="C56" s="63" t="s">
         <v>37</v>
       </c>
@@ -5650,7 +5675,7 @@
       <c r="A57" s="38">
         <v>53</v>
       </c>
-      <c r="B57" s="117"/>
+      <c r="B57" s="118"/>
       <c r="C57" s="63" t="s">
         <v>38</v>
       </c>
@@ -5704,7 +5729,7 @@
       <c r="A58" s="38">
         <v>54</v>
       </c>
-      <c r="B58" s="117"/>
+      <c r="B58" s="118"/>
       <c r="C58" s="63" t="s">
         <v>39</v>
       </c>
@@ -5758,7 +5783,7 @@
       <c r="A59" s="38">
         <v>55</v>
       </c>
-      <c r="B59" s="117"/>
+      <c r="B59" s="118"/>
       <c r="C59" s="63" t="s">
         <v>222</v>
       </c>
@@ -5812,7 +5837,7 @@
       <c r="A60" s="38">
         <v>56</v>
       </c>
-      <c r="B60" s="117"/>
+      <c r="B60" s="118"/>
       <c r="C60" s="63" t="s">
         <v>235</v>
       </c>
@@ -5866,7 +5891,7 @@
       <c r="A61" s="38">
         <v>57</v>
       </c>
-      <c r="B61" s="117"/>
+      <c r="B61" s="118"/>
       <c r="C61" s="63" t="s">
         <v>236</v>
       </c>
@@ -5920,7 +5945,7 @@
       <c r="A62" s="38">
         <v>58</v>
       </c>
-      <c r="B62" s="117"/>
+      <c r="B62" s="118"/>
       <c r="C62" s="64" t="s">
         <v>167</v>
       </c>
@@ -5974,7 +5999,7 @@
       <c r="A63" s="65">
         <v>59</v>
       </c>
-      <c r="B63" s="118"/>
+      <c r="B63" s="119"/>
       <c r="C63" s="66" t="s">
         <v>87</v>
       </c>
@@ -6025,23 +6050,23 @@
       <c r="P63" s="37"/>
     </row>
     <row r="64" spans="1:16" ht="21" x14ac:dyDescent="0.3">
-      <c r="A64" s="122" t="s">
+      <c r="A64" s="123" t="s">
         <v>40</v>
       </c>
-      <c r="B64" s="123"/>
-      <c r="C64" s="123"/>
-      <c r="D64" s="123"/>
-      <c r="E64" s="123"/>
-      <c r="F64" s="123"/>
-      <c r="G64" s="123"/>
-      <c r="H64" s="123"/>
-      <c r="I64" s="123"/>
-      <c r="J64" s="123"/>
-      <c r="K64" s="123"/>
-      <c r="L64" s="123"/>
-      <c r="M64" s="123"/>
-      <c r="N64" s="123"/>
-      <c r="O64" s="123"/>
+      <c r="B64" s="124"/>
+      <c r="C64" s="124"/>
+      <c r="D64" s="124"/>
+      <c r="E64" s="124"/>
+      <c r="F64" s="124"/>
+      <c r="G64" s="124"/>
+      <c r="H64" s="124"/>
+      <c r="I64" s="124"/>
+      <c r="J64" s="124"/>
+      <c r="K64" s="124"/>
+      <c r="L64" s="124"/>
+      <c r="M64" s="124"/>
+      <c r="N64" s="124"/>
+      <c r="O64" s="124"/>
       <c r="P64" s="70">
         <f>SUM(P5:P63)</f>
         <v>0</v>
@@ -6062,13 +6087,13 @@
       <c r="H65" s="74"/>
       <c r="I65" s="74"/>
       <c r="J65" s="73"/>
-      <c r="K65" s="124" t="s">
+      <c r="K65" s="125" t="s">
         <v>42</v>
       </c>
-      <c r="L65" s="124"/>
-      <c r="M65" s="124"/>
-      <c r="N65" s="124"/>
-      <c r="O65" s="124"/>
+      <c r="L65" s="125"/>
+      <c r="M65" s="125"/>
+      <c r="N65" s="125"/>
+      <c r="O65" s="125"/>
       <c r="P65" s="75">
         <f>P64/8</f>
         <v>0</v>
@@ -8688,10 +8713,10 @@
         <v>4</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>62</v>
+        <v>307</v>
       </c>
       <c r="D1" s="81" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>63</v>
@@ -8700,10 +8725,10 @@
         <v>64</v>
       </c>
       <c r="G1" s="81" t="s">
-        <v>178</v>
+        <v>310</v>
       </c>
       <c r="H1" s="81" t="s">
-        <v>179</v>
+        <v>309</v>
       </c>
       <c r="I1" s="19" t="s">
         <v>65</v>
@@ -8727,16 +8752,16 @@
         <v>71</v>
       </c>
       <c r="P1" s="19" t="s">
-        <v>72</v>
+        <v>308</v>
       </c>
       <c r="Q1" s="81" t="s">
-        <v>73</v>
+        <v>311</v>
       </c>
       <c r="R1" s="81" t="s">
-        <v>120</v>
+        <v>312</v>
       </c>
       <c r="S1" s="19" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -10715,7 +10740,7 @@
         <v>0</v>
       </c>
       <c r="S34" s="14">
-        <f t="shared" ref="S34:S65" si="1">SUM(C34:R34)</f>
+        <f t="shared" ref="S34:S60" si="1">SUM(C34:R34)</f>
         <v>36.1</v>
       </c>
     </row>
@@ -12294,8 +12319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12315,10 +12340,10 @@
         <v>4</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>62</v>
+        <v>307</v>
       </c>
       <c r="D1" s="81" t="s">
-        <v>92</v>
+        <v>313</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>70</v>
@@ -12327,16 +12352,16 @@
         <v>71</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>72</v>
+        <v>308</v>
       </c>
       <c r="H1" s="81" t="s">
-        <v>73</v>
+        <v>311</v>
       </c>
       <c r="I1" s="81" t="s">
         <v>302</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -14335,7 +14360,7 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -14355,13 +14380,13 @@
         <v>4</v>
       </c>
       <c r="C1" s="84" t="s">
-        <v>303</v>
-      </c>
-      <c r="D1" s="85" t="s">
+        <v>314</v>
+      </c>
+      <c r="D1" s="126" t="s">
         <v>302</v>
       </c>
-      <c r="E1" s="125" t="s">
-        <v>306</v>
+      <c r="E1" s="127" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>